<commit_message>
add some python practices
</commit_message>
<xml_diff>
--- a/Chonqqing Power Grid/整合数据14-18-0501.xlsx
+++ b/Chonqqing Power Grid/整合数据14-18-0501.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\users\chen_\git\python-practices\chonqqing power grid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\chen_\git\Python-Practices\Chonqqing Power Grid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0163911-FEBE-4A29-ACE8-88B0ADC54D11}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -736,8 +735,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -755,6 +754,15 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -796,16 +804,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -905,23 +932,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -957,23 +967,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1149,11 +1142,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1180,7 +1173,7 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -7112,11 +7105,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H230" xr:uid="{78DBB30B-A34A-4342-ACE7-6B6E55B223E4}"/>
+  <autoFilter ref="A1:H230"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>1.112474705</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>